<commit_message>
Class practice + Class Project updates
</commit_message>
<xml_diff>
--- a/projects/P2 - Retail Sales/Retail_Sales_Data.xlsx
+++ b/projects/P2 - Retail Sales/Retail_Sales_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobsteffen/Library/CloudStorage/Dropbox/Academic/BYU/Teaching/IS 303/IS 303 - 2023 Fall/Assignments/P2 - Retail Sales - Pandas and Postgres/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jackestes/Documents/Current Semester/IS303/projects/P2 - Retail Sales/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA1AF6C-E5D0-6147-A231-172AC3E58371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606964EE-831C-AB4D-A3DE-5AFC56C81C78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="1240" windowWidth="27260" windowHeight="20200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="20140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -850,10 +850,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="9" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>